<commit_message>
refatorado adicionei a classe ExcelData, Sanpshot e DriverFactory
</commit_message>
<xml_diff>
--- a/src/main/java/resources/Cadastro.xlsx
+++ b/src/main/java/resources/Cadastro.xlsx
@@ -3,17 +3,17 @@
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
   <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="21328"/>
   <workbookPr defaultThemeVersion="166925"/>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:801_{D9521D0C-BA18-4315-BAFE-EEBCA5F5F735}" xr6:coauthVersionLast="41" xr6:coauthVersionMax="41" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:801_{C792E37D-990F-45F2-A365-6F7BC89A262D}" xr6:coauthVersionLast="41" xr6:coauthVersionMax="41" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="1170" yWindow="1170" windowWidth="20790" windowHeight="11820" activeTab="2" xr2:uid="{E048A342-EB01-4E79-B803-099FC3174510}"/>
+    <workbookView xWindow="2340" yWindow="2340" windowWidth="15405" windowHeight="11340" activeTab="1" xr2:uid="{E048A342-EB01-4E79-B803-099FC3174510}"/>
   </bookViews>
   <sheets>
     <sheet name="Cadastro" sheetId="1" r:id="rId1"/>
     <sheet name="Lupa" sheetId="2" r:id="rId2"/>
     <sheet name="Home" sheetId="3" r:id="rId3"/>
   </sheets>
-  <calcPr calcId="191029"/>
-  <oleSize ref="A1:O7"/>
+  <calcPr calcId="0"/>
+  <oleSize ref="A1:L17"/>
   <extLst>
     <ext xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" uri="{140A7094-0E35-4892-8432-C4D2E57EDEB5}">
       <x15:workbookPr chartTrackingRefBase="1"/>
@@ -29,7 +29,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="27" uniqueCount="23">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="21" uniqueCount="21">
   <si>
     <t>nome</t>
   </si>
@@ -85,19 +85,13 @@
     <t>Fiji</t>
   </si>
   <si>
-    <t>Loise</t>
-  </si>
-  <si>
-    <t>numero do cartao</t>
-  </si>
-  <si>
-    <t>cvv</t>
-  </si>
-  <si>
-    <t>mês</t>
-  </si>
-  <si>
-    <t>ano</t>
+    <t>Item a ser pesquisado</t>
+  </si>
+  <si>
+    <t>HP Pavilion 15z Laptop</t>
+  </si>
+  <si>
+    <t>gggggggggg</t>
   </si>
 </sst>
 </file>
@@ -469,10 +463,10 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{174BA2E0-7519-4B50-B69F-7AD84DC24A92}">
-  <dimension ref="A1:N7"/>
+  <dimension ref="A1:J7"/>
   <sheetViews>
-    <sheetView topLeftCell="D1" workbookViewId="0">
-      <selection activeCell="K1" sqref="K1"/>
+    <sheetView workbookViewId="0">
+      <selection activeCell="A2" sqref="A2"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -486,7 +480,7 @@
     <col min="11" max="11" width="21.7109375" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:14" x14ac:dyDescent="0.25">
+    <row r="1" spans="1:10" x14ac:dyDescent="0.25">
       <c r="A1" t="s">
         <v>0</v>
       </c>
@@ -517,22 +511,10 @@
       <c r="J1" t="s">
         <v>16</v>
       </c>
-      <c r="K1" t="s">
-        <v>19</v>
-      </c>
-      <c r="L1" t="s">
+    </row>
+    <row r="2" spans="1:10" x14ac:dyDescent="0.25">
+      <c r="A2" t="s">
         <v>20</v>
-      </c>
-      <c r="M1" t="s">
-        <v>21</v>
-      </c>
-      <c r="N1" t="s">
-        <v>22</v>
-      </c>
-    </row>
-    <row r="2" spans="1:14" x14ac:dyDescent="0.25">
-      <c r="A2" t="s">
-        <v>18</v>
       </c>
       <c r="B2" t="s">
         <v>8</v>
@@ -561,33 +543,21 @@
       <c r="J2" t="s">
         <v>17</v>
       </c>
-      <c r="K2">
-        <v>928900298832</v>
-      </c>
-      <c r="L2">
-        <v>123</v>
-      </c>
-      <c r="M2">
-        <v>2</v>
-      </c>
-      <c r="N2">
-        <v>2020</v>
-      </c>
-    </row>
-    <row r="3" spans="1:14" x14ac:dyDescent="0.25">
+    </row>
+    <row r="3" spans="1:10" x14ac:dyDescent="0.25">
       <c r="C3" s="1"/>
     </row>
-    <row r="4" spans="1:14" x14ac:dyDescent="0.25">
+    <row r="4" spans="1:10" x14ac:dyDescent="0.25">
       <c r="C4" s="1"/>
     </row>
-    <row r="5" spans="1:14" x14ac:dyDescent="0.25">
+    <row r="5" spans="1:10" x14ac:dyDescent="0.25">
       <c r="C5" s="1"/>
       <c r="H5" s="2"/>
     </row>
-    <row r="6" spans="1:14" x14ac:dyDescent="0.25">
+    <row r="6" spans="1:10" x14ac:dyDescent="0.25">
       <c r="C6" s="1"/>
     </row>
-    <row r="7" spans="1:14" x14ac:dyDescent="0.25">
+    <row r="7" spans="1:10" x14ac:dyDescent="0.25">
       <c r="C7" s="1"/>
     </row>
   </sheetData>
@@ -603,99 +573,50 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{6EA487C3-8D29-44F6-BCB8-1158C33B294D}">
   <dimension ref="A1:F2"/>
   <sheetViews>
-    <sheetView workbookViewId="0">
-      <selection activeCell="F3" sqref="F3"/>
+    <sheetView tabSelected="1" workbookViewId="0">
+      <selection activeCell="A6" sqref="A6"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
   <cols>
+    <col min="1" max="1" width="24.7109375" bestFit="1" customWidth="1"/>
     <col min="3" max="3" width="16.7109375" bestFit="1" customWidth="1"/>
   </cols>
   <sheetData>
     <row r="1" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A1" t="s">
-        <v>0</v>
-      </c>
-      <c r="B1" t="s">
-        <v>14</v>
-      </c>
-      <c r="C1" t="str">
-        <f>Cadastro!K1</f>
-        <v>numero do cartao</v>
-      </c>
-      <c r="D1" t="str">
-        <f>Cadastro!L1</f>
-        <v>cvv</v>
-      </c>
-      <c r="E1" t="str">
-        <f>Cadastro!M1</f>
-        <v>mês</v>
-      </c>
-      <c r="F1" t="str">
-        <f>Cadastro!N1</f>
-        <v>ano</v>
-      </c>
+        <v>18</v>
+      </c>
+      <c r="C1" s="2"/>
+      <c r="D1" s="2"/>
+      <c r="E1" s="2"/>
+      <c r="F1" s="2"/>
     </row>
     <row r="2" spans="1:6" x14ac:dyDescent="0.25">
-      <c r="A2" t="str">
-        <f>Cadastro!A2</f>
-        <v>Loise</v>
-      </c>
-      <c r="B2" t="str">
-        <f>Cadastro!I2</f>
-        <v>Test12</v>
-      </c>
-      <c r="C2">
-        <f>Cadastro!K2</f>
-        <v>928900298832</v>
-      </c>
-      <c r="D2">
-        <f>Cadastro!L2</f>
-        <v>123</v>
-      </c>
-      <c r="E2">
-        <f>Cadastro!M2</f>
-        <v>2</v>
-      </c>
-      <c r="F2">
-        <f>Cadastro!N2</f>
-        <v>2020</v>
-      </c>
+      <c r="A2" t="s">
+        <v>19</v>
+      </c>
+      <c r="C2" s="2"/>
+      <c r="D2" s="2"/>
+      <c r="E2" s="2"/>
+      <c r="F2" s="2"/>
     </row>
   </sheetData>
   <pageMargins left="0.511811024" right="0.511811024" top="0.78740157499999996" bottom="0.78740157499999996" header="0.31496062000000002" footer="0.31496062000000002"/>
+  <pageSetup paperSize="9" orientation="portrait" r:id="rId1"/>
 </worksheet>
 </file>
 
 <file path=xl/worksheets/sheet3.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{16C14BAC-2A49-4A7D-BDD3-12907F652112}">
-  <dimension ref="A1:B2"/>
+  <dimension ref="A1"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="B2" sqref="B2"/>
+    <sheetView workbookViewId="0">
+      <selection activeCell="B2" sqref="A1:B2"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
-  <sheetData>
-    <row r="1" spans="1:2" x14ac:dyDescent="0.25">
-      <c r="A1" t="s">
-        <v>0</v>
-      </c>
-      <c r="B1" t="s">
-        <v>14</v>
-      </c>
-    </row>
-    <row r="2" spans="1:2" x14ac:dyDescent="0.25">
-      <c r="A2" t="str">
-        <f>Cadastro!A2</f>
-        <v>Loise</v>
-      </c>
-      <c r="B2" t="str">
-        <f>Cadastro!I2</f>
-        <v>Test12</v>
-      </c>
-    </row>
-  </sheetData>
+  <sheetData/>
   <pageMargins left="0.511811024" right="0.511811024" top="0.78740157499999996" bottom="0.78740157499999996" header="0.31496062000000002" footer="0.31496062000000002"/>
 </worksheet>
 </file>
</xml_diff>

<commit_message>
Refatorando o codigo Exclui classes unitilizadas e corrigi os assert dos testes positivos
</commit_message>
<xml_diff>
--- a/src/main/java/resources/Cadastro.xlsx
+++ b/src/main/java/resources/Cadastro.xlsx
@@ -3,9 +3,14 @@
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
   <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="21328"/>
   <workbookPr defaultThemeVersion="166925"/>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:801_{C792E37D-990F-45F2-A365-6F7BC89A262D}" xr6:coauthVersionLast="41" xr6:coauthVersionMax="41" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
+    <mc:Choice Requires="x15">
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\marcos.souza\Documents\Marcos\Java\Marcos\ProjetoAvaliacaoTDD\workspace\projeto\src\main\java\resources\"/>
+    </mc:Choice>
+  </mc:AlternateContent>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{477F0F4E-D315-47B7-9419-8A3C44BD2849}" xr6:coauthVersionLast="41" xr6:coauthVersionMax="41" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="2340" yWindow="2340" windowWidth="15405" windowHeight="11340" activeTab="1" xr2:uid="{E048A342-EB01-4E79-B803-099FC3174510}"/>
+    <workbookView xWindow="1950" yWindow="1950" windowWidth="15375" windowHeight="7875" xr2:uid="{E048A342-EB01-4E79-B803-099FC3174510}"/>
   </bookViews>
   <sheets>
     <sheet name="Cadastro" sheetId="1" r:id="rId1"/>
@@ -13,16 +18,9 @@
     <sheet name="Home" sheetId="3" r:id="rId3"/>
   </sheets>
   <calcPr calcId="0"/>
-  <oleSize ref="A1:L17"/>
   <extLst>
     <ext xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" uri="{140A7094-0E35-4892-8432-C4D2E57EDEB5}">
       <x15:workbookPr chartTrackingRefBase="1"/>
-    </ext>
-    <ext xmlns:xcalcf="http://schemas.microsoft.com/office/spreadsheetml/2018/calcfeatures" uri="{B58B0392-4F1F-4190-BB64-5DF3571DCE5F}">
-      <xcalcf:calcFeatures>
-        <xcalcf:feature name="microsoft.com:RD"/>
-        <xcalcf:feature name="microsoft.com:FV"/>
-      </xcalcf:calcFeatures>
     </ext>
   </extLst>
 </workbook>
@@ -55,12 +53,6 @@
     <t>cep</t>
   </si>
   <si>
-    <t>Xavier</t>
-  </si>
-  <si>
-    <t>marcos@email.com</t>
-  </si>
-  <si>
     <t>Osasco</t>
   </si>
   <si>
@@ -91,7 +83,13 @@
     <t>HP Pavilion 15z Laptop</t>
   </si>
   <si>
-    <t>gggggggggg</t>
+    <t>Sales</t>
+  </si>
+  <si>
+    <t>antsa@email.com</t>
+  </si>
+  <si>
+    <t>Jefrey</t>
   </si>
 </sst>
 </file>
@@ -465,7 +463,7 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{174BA2E0-7519-4B50-B69F-7AD84DC24A92}">
   <dimension ref="A1:J7"/>
   <sheetViews>
-    <sheetView workbookViewId="0">
+    <sheetView tabSelected="1" workbookViewId="0">
       <selection activeCell="A2" sqref="A2"/>
     </sheetView>
   </sheetViews>
@@ -506,10 +504,10 @@
         <v>7</v>
       </c>
       <c r="I1" t="s">
+        <v>12</v>
+      </c>
+      <c r="J1" t="s">
         <v>14</v>
-      </c>
-      <c r="J1" t="s">
-        <v>16</v>
       </c>
     </row>
     <row r="2" spans="1:10" x14ac:dyDescent="0.25">
@@ -517,31 +515,31 @@
         <v>20</v>
       </c>
       <c r="B2" t="s">
-        <v>8</v>
+        <v>18</v>
       </c>
       <c r="C2" s="1" t="s">
-        <v>9</v>
+        <v>19</v>
       </c>
       <c r="D2">
         <v>11977348745</v>
       </c>
       <c r="E2" t="s">
+        <v>8</v>
+      </c>
+      <c r="F2" t="s">
+        <v>11</v>
+      </c>
+      <c r="G2" t="s">
+        <v>9</v>
+      </c>
+      <c r="H2" t="s">
         <v>10</v>
       </c>
-      <c r="F2" t="s">
+      <c r="I2" t="s">
         <v>13</v>
       </c>
-      <c r="G2" t="s">
-        <v>11</v>
-      </c>
-      <c r="H2" t="s">
-        <v>12</v>
-      </c>
-      <c r="I2" t="s">
+      <c r="J2" t="s">
         <v>15</v>
-      </c>
-      <c r="J2" t="s">
-        <v>17</v>
       </c>
     </row>
     <row r="3" spans="1:10" x14ac:dyDescent="0.25">
@@ -573,8 +571,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{6EA487C3-8D29-44F6-BCB8-1158C33B294D}">
   <dimension ref="A1:F2"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="A6" sqref="A6"/>
+    <sheetView workbookViewId="0">
+      <selection activeCell="A2" sqref="A2"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -585,7 +583,7 @@
   <sheetData>
     <row r="1" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A1" t="s">
-        <v>18</v>
+        <v>16</v>
       </c>
       <c r="C1" s="2"/>
       <c r="D1" s="2"/>
@@ -594,7 +592,7 @@
     </row>
     <row r="2" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A2" t="s">
-        <v>19</v>
+        <v>17</v>
       </c>
       <c r="C2" s="2"/>
       <c r="D2" s="2"/>

</xml_diff>